<commit_message>
Add final state logic
</commit_message>
<xml_diff>
--- a/FSM.xlsx
+++ b/FSM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeanw\ise-chess-timer-schematics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD5093C4-EAF7-42FD-B1A4-EE9F269E3D6E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C61621E8-10EB-4807-8F11-4EF347AA3A52}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2232" yWindow="2232" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{D892BDF2-57BC-4D16-A2A5-408BF51F533C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{D892BDF2-57BC-4D16-A2A5-408BF51F533C}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="51">
   <si>
     <t>Y2</t>
   </si>
@@ -152,6 +152,39 @@
   </si>
   <si>
     <t>W</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>Y2\Y1 Y0</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>J = Y1'Y0</t>
+  </si>
+  <si>
+    <t>K = Y1 Y0'</t>
+  </si>
+  <si>
+    <t>Z = Y1 Y0</t>
+  </si>
+  <si>
+    <t>W = Y2</t>
   </si>
 </sst>
 </file>
@@ -278,7 +311,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -444,12 +477,141 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -505,8 +667,61 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -825,7 +1040,7 @@
   <dimension ref="A1:T58"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:P6"/>
+      <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2953,68 +3168,111 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67C0B194-84A2-491B-9690-61242E5914D6}">
-  <dimension ref="A2:H9"/>
+  <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E2" s="1" t="s">
+    <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="43" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="K2" s="56" t="s">
+        <v>42</v>
+      </c>
+      <c r="L2" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="M2" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="N2" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="O2" s="51" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="5">
-        <v>0</v>
-      </c>
-      <c r="C3" s="5">
-        <v>0</v>
-      </c>
-      <c r="D3" s="33">
-        <v>0</v>
-      </c>
-      <c r="E3" s="34">
-        <v>0</v>
-      </c>
-      <c r="F3" s="34">
-        <v>0</v>
-      </c>
-      <c r="G3" s="34">
-        <v>0</v>
-      </c>
-      <c r="H3" s="34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="B3" s="44">
+        <v>0</v>
+      </c>
+      <c r="C3" s="35">
+        <v>0</v>
+      </c>
+      <c r="D3" s="35">
+        <v>0</v>
+      </c>
+      <c r="E3" s="39">
+        <v>0</v>
+      </c>
+      <c r="F3" s="40">
+        <v>0</v>
+      </c>
+      <c r="G3" s="40">
+        <v>0</v>
+      </c>
+      <c r="H3" s="40">
+        <v>0</v>
+      </c>
+      <c r="K3" s="52">
+        <v>0</v>
+      </c>
+      <c r="L3" s="39">
+        <v>0</v>
+      </c>
+      <c r="M3" s="54">
+        <v>1</v>
+      </c>
+      <c r="N3" s="40">
+        <v>0</v>
+      </c>
+      <c r="O3" s="40">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="45">
         <v>0</v>
       </c>
       <c r="C4" s="5">
         <v>0</v>
       </c>
-      <c r="D4" s="33">
-        <v>1</v>
-      </c>
-      <c r="E4" s="34">
+      <c r="D4" s="5">
+        <v>1</v>
+      </c>
+      <c r="E4" s="33">
         <v>1</v>
       </c>
       <c r="F4" s="34">
@@ -3026,21 +3284,36 @@
       <c r="H4" s="34">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="K4" s="53">
+        <v>1</v>
+      </c>
+      <c r="L4" s="33">
+        <v>0</v>
+      </c>
+      <c r="M4" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="O4" s="34" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="45">
         <v>0</v>
       </c>
       <c r="C5" s="5">
         <v>1</v>
       </c>
-      <c r="D5" s="33">
-        <v>0</v>
-      </c>
-      <c r="E5" s="34">
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="33">
         <v>0</v>
       </c>
       <c r="F5" s="34">
@@ -3053,20 +3326,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="45">
         <v>0</v>
       </c>
       <c r="C6" s="5">
         <v>1</v>
       </c>
-      <c r="D6" s="33">
-        <v>1</v>
-      </c>
-      <c r="E6" s="34">
+      <c r="D6" s="5">
+        <v>1</v>
+      </c>
+      <c r="E6" s="33">
         <v>0</v>
       </c>
       <c r="F6" s="34">
@@ -3079,20 +3352,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="45">
         <v>1</v>
       </c>
       <c r="C7" s="5">
         <v>0</v>
       </c>
-      <c r="D7" s="33">
-        <v>0</v>
-      </c>
-      <c r="E7" s="34">
+      <c r="D7" s="5">
+        <v>0</v>
+      </c>
+      <c r="E7" s="33">
         <v>0</v>
       </c>
       <c r="F7" s="34">
@@ -3104,9 +3377,244 @@
       <c r="H7" s="34">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F9" s="9"/>
+      <c r="K7" s="56" t="s">
+        <v>42</v>
+      </c>
+      <c r="L7" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="M7" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="N7" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="O7" s="51" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="45">
+        <v>1</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5">
+        <v>1</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="52">
+        <v>0</v>
+      </c>
+      <c r="L8" s="57">
+        <v>0</v>
+      </c>
+      <c r="M8" s="58">
+        <v>0</v>
+      </c>
+      <c r="N8" s="58">
+        <v>0</v>
+      </c>
+      <c r="O8" s="54">
+        <v>1</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="45">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0</v>
+      </c>
+      <c r="E9" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="53">
+        <v>1</v>
+      </c>
+      <c r="L9" s="59">
+        <v>0</v>
+      </c>
+      <c r="M9" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="N9" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="O9" s="55" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="45">
+        <v>1</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5">
+        <v>1</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="34" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K12" s="56" t="s">
+        <v>42</v>
+      </c>
+      <c r="L12" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="M12" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="N12" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="O12" s="51" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="K13" s="52">
+        <v>0</v>
+      </c>
+      <c r="L13" s="57">
+        <v>0</v>
+      </c>
+      <c r="M13" s="58">
+        <v>0</v>
+      </c>
+      <c r="N13" s="54">
+        <v>1</v>
+      </c>
+      <c r="O13" s="58">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K14" s="53">
+        <v>1</v>
+      </c>
+      <c r="L14" s="59">
+        <v>0</v>
+      </c>
+      <c r="M14" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="N14" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="O14" s="60" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S16" s="9"/>
+    </row>
+    <row r="17" spans="11:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K17" s="56" t="s">
+        <v>42</v>
+      </c>
+      <c r="L17" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="M17" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="N17" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="O17" s="51" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="11:17" x14ac:dyDescent="0.3">
+      <c r="K18" s="52">
+        <v>0</v>
+      </c>
+      <c r="L18" s="57">
+        <v>0</v>
+      </c>
+      <c r="M18" s="58">
+        <v>0</v>
+      </c>
+      <c r="N18" s="58">
+        <v>0</v>
+      </c>
+      <c r="O18" s="58">
+        <v>0</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="11:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K19" s="53">
+        <v>1</v>
+      </c>
+      <c r="L19" s="61">
+        <v>1</v>
+      </c>
+      <c r="M19" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="N19" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="O19" s="55" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Add Proteus project to test FSM
</commit_message>
<xml_diff>
--- a/FSM.xlsx
+++ b/FSM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeanw\ise-chess-timer-schematics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C61621E8-10EB-4807-8F11-4EF347AA3A52}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C7E531-AE92-4BC5-AADF-1E2764FAAC2B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{D892BDF2-57BC-4D16-A2A5-408BF51F533C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D892BDF2-57BC-4D16-A2A5-408BF51F533C}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -139,9 +139,6 @@
     <t>Y1'*Y0*BUT + Y0*TIM*BUT' + Y0*CHQ*BUT' + Y1*CHQ'*TIM'*BUT'</t>
   </si>
   <si>
-    <t>Y0*BUT' + Y2'*Y1'*CHQ*BUT + Y2'*Y1'*TIM*BUT + Y2'*Y0'*CHQ'*TIM'*BUT'</t>
-  </si>
-  <si>
     <t>J</t>
   </si>
   <si>
@@ -185,6 +182,9 @@
   </si>
   <si>
     <t>W = Y2</t>
+  </si>
+  <si>
+    <t>Y0*BUT' + Y2'*Y1'*CHQ*BUT + Y2'*Y1'*TIM*BUT + Y2'*Y0'*CHQ'*TIM'*BUT</t>
   </si>
 </sst>
 </file>
@@ -229,18 +229,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="12">
@@ -609,7 +609,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -659,8 +659,7 @@
     <xf numFmtId="0" fontId="4" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -722,6 +721,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -1037,22 +1037,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A4C429B-746C-4748-8FEA-F2B51B7B4385}">
-  <dimension ref="A1:T58"/>
+  <dimension ref="A1:S64"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="T19" sqref="T19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="7" max="7" width="4.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="38.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="65.109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="3" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="42.21875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="65.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>9</v>
       </c>
@@ -1072,7 +1074,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1103,24 +1105,12 @@
       <c r="K2" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N2" s="5">
-        <v>0</v>
-      </c>
-      <c r="O2" s="5">
-        <v>0</v>
-      </c>
-      <c r="P2" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" s="32">
-        <v>0</v>
-      </c>
-      <c r="B3" s="27">
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="31">
+        <v>0</v>
+      </c>
+      <c r="B3" s="26">
         <v>0</v>
       </c>
       <c r="C3" s="22">
@@ -1150,24 +1140,15 @@
       <c r="K3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N3" s="5">
-        <v>0</v>
-      </c>
-      <c r="O3" s="5">
-        <v>0</v>
-      </c>
-      <c r="P3" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" s="32">
-        <v>1</v>
-      </c>
-      <c r="B4" s="28">
+      <c r="M3" s="25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="31">
+        <v>1</v>
+      </c>
+      <c r="B4" s="27">
         <v>0</v>
       </c>
       <c r="C4" s="19">
@@ -1197,24 +1178,21 @@
       <c r="K4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N4" s="5">
-        <v>0</v>
-      </c>
-      <c r="O4" s="5">
-        <v>1</v>
-      </c>
-      <c r="P4" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A5" s="32">
+      <c r="M4" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="N4" s="61" t="s">
+        <v>28</v>
+      </c>
+      <c r="O4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="31">
         <v>2</v>
       </c>
-      <c r="B5" s="29">
+      <c r="B5" s="28">
         <v>0</v>
       </c>
       <c r="C5" s="23">
@@ -1244,24 +1222,21 @@
       <c r="K5" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N5" s="5">
-        <v>0</v>
-      </c>
-      <c r="O5" s="5">
-        <v>1</v>
-      </c>
-      <c r="P5" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A6" s="32">
+      <c r="M5" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="N5" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="O5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="31">
         <v>3</v>
       </c>
-      <c r="B6" s="28">
+      <c r="B6" s="27">
         <v>0</v>
       </c>
       <c r="C6" s="19">
@@ -1291,24 +1266,21 @@
       <c r="K6" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="M6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N6" s="5">
-        <v>1</v>
-      </c>
-      <c r="O6" s="5">
-        <v>0</v>
-      </c>
-      <c r="P6" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7" s="32">
+      <c r="M6" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="N6" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="O6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" s="31">
         <v>4</v>
       </c>
-      <c r="B7" s="29">
+      <c r="B7" s="28">
         <v>0</v>
       </c>
       <c r="C7" s="23">
@@ -1339,11 +1311,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A8" s="32">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8" s="31">
         <v>5</v>
       </c>
-      <c r="B8" s="28">
+      <c r="B8" s="27">
         <v>0</v>
       </c>
       <c r="C8" s="19">
@@ -1374,11 +1346,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A9" s="32">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A9" s="31">
         <v>6</v>
       </c>
-      <c r="B9" s="29">
+      <c r="B9" s="28">
         <v>0</v>
       </c>
       <c r="C9" s="23">
@@ -1409,11 +1381,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="32">
+    <row r="10" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="31">
         <v>7</v>
       </c>
-      <c r="B10" s="30">
+      <c r="B10" s="29">
         <v>0</v>
       </c>
       <c r="C10" s="20">
@@ -1445,11 +1417,11 @@
       </c>
       <c r="S10" s="9"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A11" s="32">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11" s="31">
         <v>8</v>
       </c>
-      <c r="B11" s="27">
+      <c r="B11" s="26">
         <v>0</v>
       </c>
       <c r="C11" s="22">
@@ -1480,11 +1452,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A12" s="32">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A12" s="31">
         <v>9</v>
       </c>
-      <c r="B12" s="28">
+      <c r="B12" s="27">
         <v>0</v>
       </c>
       <c r="C12" s="19">
@@ -1514,15 +1486,12 @@
       <c r="K12" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="R12" s="26" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" ht="18" x14ac:dyDescent="0.35">
-      <c r="A13" s="32">
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A13" s="31">
         <v>10</v>
       </c>
-      <c r="B13" s="29">
+      <c r="B13" s="28">
         <v>0</v>
       </c>
       <c r="C13" s="23">
@@ -1552,21 +1521,12 @@
       <c r="K13" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="R13" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="S13" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="T13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" ht="18" x14ac:dyDescent="0.35">
-      <c r="A14" s="32">
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A14" s="31">
         <v>11</v>
       </c>
-      <c r="B14" s="28">
+      <c r="B14" s="27">
         <v>0</v>
       </c>
       <c r="C14" s="19">
@@ -1596,21 +1556,12 @@
       <c r="K14" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="R14" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="S14" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="T14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" ht="18" x14ac:dyDescent="0.35">
-      <c r="A15" s="32">
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A15" s="31">
         <v>12</v>
       </c>
-      <c r="B15" s="29">
+      <c r="B15" s="28">
         <v>0</v>
       </c>
       <c r="C15" s="23">
@@ -1640,21 +1591,12 @@
       <c r="K15" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="R15" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="S15" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="T15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A16" s="32">
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A16" s="31">
         <v>13</v>
       </c>
-      <c r="B16" s="28">
+      <c r="B16" s="27">
         <v>0</v>
       </c>
       <c r="C16" s="19">
@@ -1686,10 +1628,10 @@
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A17" s="32">
-        <v>14</v>
-      </c>
-      <c r="B17" s="29">
+      <c r="A17" s="31">
+        <v>14</v>
+      </c>
+      <c r="B17" s="28">
         <v>0</v>
       </c>
       <c r="C17" s="23">
@@ -1721,10 +1663,10 @@
       </c>
     </row>
     <row r="18" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="32">
+      <c r="A18" s="31">
         <v>15</v>
       </c>
-      <c r="B18" s="30">
+      <c r="B18" s="29">
         <v>0</v>
       </c>
       <c r="C18" s="20">
@@ -1756,10 +1698,10 @@
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A19" s="32">
+      <c r="A19" s="31">
         <v>16</v>
       </c>
-      <c r="B19" s="27">
+      <c r="B19" s="26">
         <v>0</v>
       </c>
       <c r="C19" s="22">
@@ -1792,10 +1734,10 @@
       <c r="S19" s="9"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A20" s="32">
+      <c r="A20" s="31">
         <v>17</v>
       </c>
-      <c r="B20" s="28">
+      <c r="B20" s="27">
         <v>0</v>
       </c>
       <c r="C20" s="19">
@@ -1828,10 +1770,10 @@
       <c r="S20" s="9"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A21" s="32">
+      <c r="A21" s="31">
         <v>18</v>
       </c>
-      <c r="B21" s="29">
+      <c r="B21" s="28">
         <v>0</v>
       </c>
       <c r="C21" s="23">
@@ -1863,10 +1805,10 @@
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A22" s="32">
+      <c r="A22" s="31">
         <v>19</v>
       </c>
-      <c r="B22" s="28">
+      <c r="B22" s="27">
         <v>0</v>
       </c>
       <c r="C22" s="19">
@@ -1898,10 +1840,10 @@
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A23" s="32">
+      <c r="A23" s="31">
         <v>20</v>
       </c>
-      <c r="B23" s="29">
+      <c r="B23" s="28">
         <v>0</v>
       </c>
       <c r="C23" s="23">
@@ -1933,10 +1875,10 @@
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A24" s="32">
+      <c r="A24" s="31">
         <v>21</v>
       </c>
-      <c r="B24" s="28">
+      <c r="B24" s="27">
         <v>0</v>
       </c>
       <c r="C24" s="19">
@@ -1968,10 +1910,10 @@
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A25" s="32">
+      <c r="A25" s="31">
         <v>22</v>
       </c>
-      <c r="B25" s="29">
+      <c r="B25" s="28">
         <v>0</v>
       </c>
       <c r="C25" s="23">
@@ -2003,10 +1945,10 @@
       </c>
     </row>
     <row r="26" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="32">
+      <c r="A26" s="31">
         <v>23</v>
       </c>
-      <c r="B26" s="30">
+      <c r="B26" s="29">
         <v>0</v>
       </c>
       <c r="C26" s="20">
@@ -2038,10 +1980,10 @@
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A27" s="32">
+      <c r="A27" s="31">
         <v>24</v>
       </c>
-      <c r="B27" s="27">
+      <c r="B27" s="26">
         <v>0</v>
       </c>
       <c r="C27" s="22">
@@ -2073,10 +2015,10 @@
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A28" s="32">
+      <c r="A28" s="31">
         <v>25</v>
       </c>
-      <c r="B28" s="28">
+      <c r="B28" s="27">
         <v>0</v>
       </c>
       <c r="C28" s="19">
@@ -2108,10 +2050,10 @@
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A29" s="32">
+      <c r="A29" s="31">
         <v>26</v>
       </c>
-      <c r="B29" s="29">
+      <c r="B29" s="28">
         <v>0</v>
       </c>
       <c r="C29" s="23">
@@ -2143,10 +2085,10 @@
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A30" s="32">
+      <c r="A30" s="31">
         <v>27</v>
       </c>
-      <c r="B30" s="28">
+      <c r="B30" s="27">
         <v>0</v>
       </c>
       <c r="C30" s="19">
@@ -2178,10 +2120,10 @@
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A31" s="32">
+      <c r="A31" s="31">
         <v>28</v>
       </c>
-      <c r="B31" s="29">
+      <c r="B31" s="28">
         <v>0</v>
       </c>
       <c r="C31" s="23">
@@ -2213,10 +2155,10 @@
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A32" s="32">
+      <c r="A32" s="31">
         <v>29</v>
       </c>
-      <c r="B32" s="28">
+      <c r="B32" s="27">
         <v>0</v>
       </c>
       <c r="C32" s="19">
@@ -2248,10 +2190,10 @@
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A33" s="32">
+      <c r="A33" s="31">
         <v>30</v>
       </c>
-      <c r="B33" s="29">
+      <c r="B33" s="28">
         <v>0</v>
       </c>
       <c r="C33" s="23">
@@ -2283,10 +2225,10 @@
       </c>
     </row>
     <row r="34" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="32">
+      <c r="A34" s="31">
         <v>31</v>
       </c>
-      <c r="B34" s="30">
+      <c r="B34" s="29">
         <v>0</v>
       </c>
       <c r="C34" s="20">
@@ -2318,10 +2260,10 @@
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A35" s="32">
+      <c r="A35" s="31">
         <v>32</v>
       </c>
-      <c r="B35" s="27">
+      <c r="B35" s="26">
         <v>1</v>
       </c>
       <c r="C35" s="22">
@@ -2353,10 +2295,10 @@
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A36" s="32">
+      <c r="A36" s="31">
         <v>33</v>
       </c>
-      <c r="B36" s="28">
+      <c r="B36" s="27">
         <v>1</v>
       </c>
       <c r="C36" s="19">
@@ -2388,10 +2330,10 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A37" s="32">
+      <c r="A37" s="31">
         <v>34</v>
       </c>
-      <c r="B37" s="29">
+      <c r="B37" s="28">
         <v>1</v>
       </c>
       <c r="C37" s="23">
@@ -2423,10 +2365,10 @@
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A38" s="32">
+      <c r="A38" s="31">
         <v>35</v>
       </c>
-      <c r="B38" s="28">
+      <c r="B38" s="27">
         <v>1</v>
       </c>
       <c r="C38" s="19">
@@ -2458,10 +2400,10 @@
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A39" s="32">
+      <c r="A39" s="31">
         <v>36</v>
       </c>
-      <c r="B39" s="29">
+      <c r="B39" s="28">
         <v>1</v>
       </c>
       <c r="C39" s="23">
@@ -2493,10 +2435,10 @@
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A40" s="32">
+      <c r="A40" s="31">
         <v>37</v>
       </c>
-      <c r="B40" s="28">
+      <c r="B40" s="27">
         <v>1</v>
       </c>
       <c r="C40" s="19">
@@ -2528,10 +2470,10 @@
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A41" s="32">
+      <c r="A41" s="31">
         <v>38</v>
       </c>
-      <c r="B41" s="29">
+      <c r="B41" s="28">
         <v>1</v>
       </c>
       <c r="C41" s="23">
@@ -2563,10 +2505,10 @@
       </c>
     </row>
     <row r="42" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="32">
+      <c r="A42" s="31">
         <v>39</v>
       </c>
-      <c r="B42" s="31">
+      <c r="B42" s="30">
         <v>1</v>
       </c>
       <c r="C42" s="21">
@@ -2598,10 +2540,10 @@
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A43" s="32">
+      <c r="A43" s="31">
         <v>40</v>
       </c>
-      <c r="B43" s="27">
+      <c r="B43" s="26">
         <v>1</v>
       </c>
       <c r="C43" s="22">
@@ -2633,10 +2575,10 @@
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A44" s="32">
+      <c r="A44" s="31">
         <v>41</v>
       </c>
-      <c r="B44" s="28">
+      <c r="B44" s="27">
         <v>1</v>
       </c>
       <c r="C44" s="19">
@@ -2668,10 +2610,10 @@
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A45" s="32">
+      <c r="A45" s="31">
         <v>42</v>
       </c>
-      <c r="B45" s="29">
+      <c r="B45" s="28">
         <v>1</v>
       </c>
       <c r="C45" s="23">
@@ -2703,10 +2645,10 @@
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A46" s="32">
+      <c r="A46" s="31">
         <v>43</v>
       </c>
-      <c r="B46" s="28">
+      <c r="B46" s="27">
         <v>1</v>
       </c>
       <c r="C46" s="19">
@@ -2738,10 +2680,10 @@
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A47" s="32">
+      <c r="A47" s="31">
         <v>44</v>
       </c>
-      <c r="B47" s="29">
+      <c r="B47" s="28">
         <v>1</v>
       </c>
       <c r="C47" s="23">
@@ -2773,10 +2715,10 @@
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A48" s="32">
+      <c r="A48" s="31">
         <v>45</v>
       </c>
-      <c r="B48" s="28">
+      <c r="B48" s="27">
         <v>1</v>
       </c>
       <c r="C48" s="19">
@@ -2808,10 +2750,10 @@
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A49" s="32">
+      <c r="A49" s="31">
         <v>46</v>
       </c>
-      <c r="B49" s="29">
+      <c r="B49" s="28">
         <v>1</v>
       </c>
       <c r="C49" s="23">
@@ -2843,10 +2785,10 @@
       </c>
     </row>
     <row r="50" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="32">
+      <c r="A50" s="31">
         <v>47</v>
       </c>
-      <c r="B50" s="30">
+      <c r="B50" s="29">
         <v>1</v>
       </c>
       <c r="C50" s="20">
@@ -2878,10 +2820,10 @@
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A51" s="32">
+      <c r="A51" s="31">
         <v>48</v>
       </c>
-      <c r="B51" s="27">
+      <c r="B51" s="26">
         <v>1</v>
       </c>
       <c r="C51" s="22">
@@ -2913,10 +2855,10 @@
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A52" s="32">
+      <c r="A52" s="31">
         <v>49</v>
       </c>
-      <c r="B52" s="28">
+      <c r="B52" s="27">
         <v>1</v>
       </c>
       <c r="C52" s="19">
@@ -2948,10 +2890,10 @@
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A53" s="32">
+      <c r="A53" s="31">
         <v>50</v>
       </c>
-      <c r="B53" s="29">
+      <c r="B53" s="28">
         <v>1</v>
       </c>
       <c r="C53" s="23">
@@ -2983,10 +2925,10 @@
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A54" s="32">
+      <c r="A54" s="31">
         <v>51</v>
       </c>
-      <c r="B54" s="28">
+      <c r="B54" s="27">
         <v>1</v>
       </c>
       <c r="C54" s="19">
@@ -3018,10 +2960,10 @@
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A55" s="32">
+      <c r="A55" s="31">
         <v>52</v>
       </c>
-      <c r="B55" s="29">
+      <c r="B55" s="28">
         <v>1</v>
       </c>
       <c r="C55" s="23">
@@ -3053,10 +2995,10 @@
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A56" s="32">
+      <c r="A56" s="31">
         <v>53</v>
       </c>
-      <c r="B56" s="28">
+      <c r="B56" s="27">
         <v>1</v>
       </c>
       <c r="C56" s="19">
@@ -3088,10 +3030,10 @@
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A57" s="32">
+      <c r="A57" s="31">
         <v>54</v>
       </c>
-      <c r="B57" s="29">
+      <c r="B57" s="28">
         <v>1</v>
       </c>
       <c r="C57" s="23">
@@ -3123,10 +3065,10 @@
       </c>
     </row>
     <row r="58" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="32">
+      <c r="A58" s="31">
         <v>55</v>
       </c>
-      <c r="B58" s="30">
+      <c r="B58" s="29">
         <v>1</v>
       </c>
       <c r="C58" s="20">
@@ -3155,11 +3097,81 @@
       </c>
       <c r="K58" s="17" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B60" s="5">
+        <v>0</v>
+      </c>
+      <c r="C60" s="5">
+        <v>0</v>
+      </c>
+      <c r="D60" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B61" s="5">
+        <v>0</v>
+      </c>
+      <c r="C61" s="5">
+        <v>0</v>
+      </c>
+      <c r="D61" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B62" s="5">
+        <v>0</v>
+      </c>
+      <c r="C62" s="5">
+        <v>1</v>
+      </c>
+      <c r="D62" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B63" s="5">
+        <v>0</v>
+      </c>
+      <c r="C63" s="5">
+        <v>1</v>
+      </c>
+      <c r="D63" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B64" s="5">
+        <v>1</v>
+      </c>
+      <c r="C64" s="5">
+        <v>0</v>
+      </c>
+      <c r="D64" s="5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="R12" r:id="rId1" display="http://www.32x8.com/" xr:uid="{46987D7C-9D83-4F55-A4FB-FD555767C20F}"/>
+    <hyperlink ref="M3" r:id="rId1" display="http://www.32x8.com/" xr:uid="{46987D7C-9D83-4F55-A4FB-FD555767C20F}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId2"/>
@@ -3170,319 +3182,319 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67C0B194-84A2-491B-9690-61242E5914D6}">
   <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="38" t="s">
+      <c r="B2" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="41" t="s">
+      <c r="E2" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="42" t="s">
+      <c r="G2" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="42" t="s">
+      <c r="H2" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="43" t="s">
+      <c r="K2" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="M2" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="N2" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="O2" s="50" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="43">
+        <v>0</v>
+      </c>
+      <c r="C3" s="34">
+        <v>0</v>
+      </c>
+      <c r="D3" s="34">
+        <v>0</v>
+      </c>
+      <c r="E3" s="38">
+        <v>0</v>
+      </c>
+      <c r="F3" s="39">
+        <v>0</v>
+      </c>
+      <c r="G3" s="39">
+        <v>0</v>
+      </c>
+      <c r="H3" s="39">
+        <v>0</v>
+      </c>
+      <c r="K3" s="51">
+        <v>0</v>
+      </c>
+      <c r="L3" s="38">
+        <v>0</v>
+      </c>
+      <c r="M3" s="53">
+        <v>1</v>
+      </c>
+      <c r="N3" s="39">
+        <v>0</v>
+      </c>
+      <c r="O3" s="39">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="44">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1</v>
+      </c>
+      <c r="E4" s="32">
+        <v>1</v>
+      </c>
+      <c r="F4" s="33">
+        <v>0</v>
+      </c>
+      <c r="G4" s="33">
+        <v>0</v>
+      </c>
+      <c r="H4" s="33">
+        <v>0</v>
+      </c>
+      <c r="K4" s="52">
+        <v>1</v>
+      </c>
+      <c r="L4" s="32">
+        <v>0</v>
+      </c>
+      <c r="M4" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="O4" s="33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="44">
+        <v>0</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="32">
+        <v>0</v>
+      </c>
+      <c r="F5" s="33">
+        <v>1</v>
+      </c>
+      <c r="G5" s="33">
+        <v>0</v>
+      </c>
+      <c r="H5" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="44">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5">
+        <v>1</v>
+      </c>
+      <c r="E6" s="32">
+        <v>0</v>
+      </c>
+      <c r="F6" s="33">
+        <v>0</v>
+      </c>
+      <c r="G6" s="33">
+        <v>1</v>
+      </c>
+      <c r="H6" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="44">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0</v>
+      </c>
+      <c r="E7" s="32">
+        <v>0</v>
+      </c>
+      <c r="F7" s="33">
+        <v>0</v>
+      </c>
+      <c r="G7" s="33">
+        <v>0</v>
+      </c>
+      <c r="H7" s="33">
+        <v>1</v>
+      </c>
+      <c r="K7" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="L7" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="M7" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="N7" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="O7" s="50" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="44">
+        <v>1</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5">
+        <v>1</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="51">
+        <v>0</v>
+      </c>
+      <c r="L8" s="56">
+        <v>0</v>
+      </c>
+      <c r="M8" s="57">
+        <v>0</v>
+      </c>
+      <c r="N8" s="57">
+        <v>0</v>
+      </c>
+      <c r="O8" s="53">
+        <v>1</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="K2" s="56" t="s">
-        <v>42</v>
-      </c>
-      <c r="L2" s="49" t="s">
-        <v>43</v>
-      </c>
-      <c r="M2" s="50" t="s">
-        <v>44</v>
-      </c>
-      <c r="N2" s="50" t="s">
-        <v>45</v>
-      </c>
-      <c r="O2" s="51" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="44">
-        <v>0</v>
-      </c>
-      <c r="C3" s="35">
-        <v>0</v>
-      </c>
-      <c r="D3" s="35">
-        <v>0</v>
-      </c>
-      <c r="E3" s="39">
-        <v>0</v>
-      </c>
-      <c r="F3" s="40">
-        <v>0</v>
-      </c>
-      <c r="G3" s="40">
-        <v>0</v>
-      </c>
-      <c r="H3" s="40">
-        <v>0</v>
-      </c>
-      <c r="K3" s="52">
-        <v>0</v>
-      </c>
-      <c r="L3" s="39">
-        <v>0</v>
-      </c>
-      <c r="M3" s="54">
-        <v>1</v>
-      </c>
-      <c r="N3" s="40">
-        <v>0</v>
-      </c>
-      <c r="O3" s="40">
-        <v>0</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="45">
-        <v>0</v>
-      </c>
-      <c r="C4" s="5">
-        <v>0</v>
-      </c>
-      <c r="D4" s="5">
-        <v>1</v>
-      </c>
-      <c r="E4" s="33">
-        <v>1</v>
-      </c>
-      <c r="F4" s="34">
-        <v>0</v>
-      </c>
-      <c r="G4" s="34">
-        <v>0</v>
-      </c>
-      <c r="H4" s="34">
-        <v>0</v>
-      </c>
-      <c r="K4" s="53">
-        <v>1</v>
-      </c>
-      <c r="L4" s="33">
-        <v>0</v>
-      </c>
-      <c r="M4" s="55" t="s">
-        <v>14</v>
-      </c>
-      <c r="N4" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="O4" s="34" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="47" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="45">
-        <v>0</v>
-      </c>
-      <c r="C5" s="5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="5">
-        <v>0</v>
-      </c>
-      <c r="E5" s="33">
-        <v>0</v>
-      </c>
-      <c r="F5" s="34">
-        <v>1</v>
-      </c>
-      <c r="G5" s="34">
-        <v>0</v>
-      </c>
-      <c r="H5" s="34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="45">
-        <v>0</v>
-      </c>
-      <c r="C6" s="5">
-        <v>1</v>
-      </c>
-      <c r="D6" s="5">
-        <v>1</v>
-      </c>
-      <c r="E6" s="33">
-        <v>0</v>
-      </c>
-      <c r="F6" s="34">
-        <v>0</v>
-      </c>
-      <c r="G6" s="34">
-        <v>1</v>
-      </c>
-      <c r="H6" s="34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="47" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="45">
-        <v>1</v>
-      </c>
-      <c r="C7" s="5">
-        <v>0</v>
-      </c>
-      <c r="D7" s="5">
-        <v>0</v>
-      </c>
-      <c r="E7" s="33">
-        <v>0</v>
-      </c>
-      <c r="F7" s="34">
-        <v>0</v>
-      </c>
-      <c r="G7" s="34">
-        <v>0</v>
-      </c>
-      <c r="H7" s="34">
-        <v>1</v>
-      </c>
-      <c r="K7" s="56" t="s">
-        <v>42</v>
-      </c>
-      <c r="L7" s="49" t="s">
-        <v>43</v>
-      </c>
-      <c r="M7" s="50" t="s">
-        <v>44</v>
-      </c>
-      <c r="N7" s="50" t="s">
-        <v>45</v>
-      </c>
-      <c r="O7" s="51" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="45">
-        <v>1</v>
-      </c>
-      <c r="C8" s="5">
-        <v>0</v>
-      </c>
-      <c r="D8" s="5">
-        <v>1</v>
-      </c>
-      <c r="E8" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="K8" s="52">
-        <v>0</v>
-      </c>
-      <c r="L8" s="57">
-        <v>0</v>
-      </c>
-      <c r="M8" s="58">
-        <v>0</v>
-      </c>
-      <c r="N8" s="58">
-        <v>0</v>
-      </c>
-      <c r="O8" s="54">
-        <v>1</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="47" t="s">
+      <c r="B9" s="44">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="52">
+        <v>1</v>
+      </c>
+      <c r="L9" s="58">
+        <v>0</v>
+      </c>
+      <c r="M9" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="N9" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="O9" s="54" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="45">
-        <v>1</v>
-      </c>
-      <c r="C9" s="5">
-        <v>1</v>
-      </c>
-      <c r="D9" s="5">
-        <v>0</v>
-      </c>
-      <c r="E9" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="K9" s="53">
-        <v>1</v>
-      </c>
-      <c r="L9" s="59">
-        <v>0</v>
-      </c>
-      <c r="M9" s="60" t="s">
-        <v>14</v>
-      </c>
-      <c r="N9" s="60" t="s">
-        <v>14</v>
-      </c>
-      <c r="O9" s="55" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="48" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="45">
+      <c r="B10" s="44">
         <v>1</v>
       </c>
       <c r="C10" s="5">
@@ -3491,71 +3503,71 @@
       <c r="D10" s="5">
         <v>1</v>
       </c>
-      <c r="E10" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="34" t="s">
+      <c r="E10" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="33" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="12" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K12" s="56" t="s">
+      <c r="K12" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="L12" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="L12" s="49" t="s">
+      <c r="M12" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="M12" s="50" t="s">
+      <c r="N12" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="N12" s="50" t="s">
+      <c r="O12" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="O12" s="51" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="K13" s="52">
-        <v>0</v>
-      </c>
-      <c r="L13" s="57">
-        <v>0</v>
-      </c>
-      <c r="M13" s="58">
-        <v>0</v>
-      </c>
-      <c r="N13" s="54">
-        <v>1</v>
-      </c>
-      <c r="O13" s="58">
+      <c r="K13" s="51">
+        <v>0</v>
+      </c>
+      <c r="L13" s="56">
+        <v>0</v>
+      </c>
+      <c r="M13" s="57">
+        <v>0</v>
+      </c>
+      <c r="N13" s="53">
+        <v>1</v>
+      </c>
+      <c r="O13" s="57">
         <v>0</v>
       </c>
       <c r="Q13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K14" s="53">
-        <v>1</v>
-      </c>
-      <c r="L14" s="59">
-        <v>0</v>
-      </c>
-      <c r="M14" s="60" t="s">
-        <v>14</v>
-      </c>
-      <c r="N14" s="55" t="s">
-        <v>14</v>
-      </c>
-      <c r="O14" s="60" t="s">
+      <c r="K14" s="52">
+        <v>1</v>
+      </c>
+      <c r="L14" s="58">
+        <v>0</v>
+      </c>
+      <c r="M14" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="N14" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="O14" s="59" t="s">
         <v>14</v>
       </c>
     </row>
@@ -3563,56 +3575,56 @@
       <c r="S16" s="9"/>
     </row>
     <row r="17" spans="11:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K17" s="56" t="s">
+      <c r="K17" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="L17" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="L17" s="49" t="s">
+      <c r="M17" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="M17" s="50" t="s">
+      <c r="N17" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="N17" s="50" t="s">
+      <c r="O17" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="O17" s="51" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="18" spans="11:17" x14ac:dyDescent="0.3">
-      <c r="K18" s="52">
-        <v>0</v>
-      </c>
-      <c r="L18" s="57">
-        <v>0</v>
-      </c>
-      <c r="M18" s="58">
-        <v>0</v>
-      </c>
-      <c r="N18" s="58">
-        <v>0</v>
-      </c>
-      <c r="O18" s="58">
+      <c r="K18" s="51">
+        <v>0</v>
+      </c>
+      <c r="L18" s="56">
+        <v>0</v>
+      </c>
+      <c r="M18" s="57">
+        <v>0</v>
+      </c>
+      <c r="N18" s="57">
+        <v>0</v>
+      </c>
+      <c r="O18" s="57">
         <v>0</v>
       </c>
       <c r="Q18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="11:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K19" s="53">
-        <v>1</v>
-      </c>
-      <c r="L19" s="61">
-        <v>1</v>
-      </c>
-      <c r="M19" s="55" t="s">
-        <v>14</v>
-      </c>
-      <c r="N19" s="55" t="s">
-        <v>14</v>
-      </c>
-      <c r="O19" s="55" t="s">
+      <c r="K19" s="52">
+        <v>1</v>
+      </c>
+      <c r="L19" s="60">
+        <v>1</v>
+      </c>
+      <c r="M19" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="N19" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="O19" s="54" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Create new FSM to prevent early timeout condition
</commit_message>
<xml_diff>
--- a/FSM.xlsx
+++ b/FSM.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeanw\ise-chess-timer-schematics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C7E531-AE92-4BC5-AADF-1E2764FAAC2B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{179AEE4E-65CD-4A78-8890-094771D66FC2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D892BDF2-57BC-4D16-A2A5-408BF51F533C}"/>
+    <workbookView xWindow="2928" yWindow="2928" windowWidth="17280" windowHeight="8964" activeTab="3" xr2:uid="{D892BDF2-57BC-4D16-A2A5-408BF51F533C}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
     <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
+    <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
+    <sheet name="Planilha4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="70">
   <si>
     <t>Y2</t>
   </si>
@@ -185,13 +187,70 @@
   </si>
   <si>
     <t>Y0*BUT' + Y2'*Y1'*CHQ*BUT + Y2'*Y1'*TIM*BUT + Y2'*Y0'*CHQ'*TIM'*BUT</t>
+  </si>
+  <si>
+    <t>PREPARATION</t>
+  </si>
+  <si>
+    <t>IDLE</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P1 LOSS</t>
+  </si>
+  <si>
+    <t>P2 LOSS</t>
+  </si>
+  <si>
+    <t>RESET</t>
+  </si>
+  <si>
+    <t>PREP</t>
+  </si>
+  <si>
+    <t>Y1 = B'CF + AB'F + A'BD'E'</t>
+  </si>
+  <si>
+    <t>Y2 = AB' + A'BE + A'BD</t>
+  </si>
+  <si>
+    <t>J = A'C'</t>
+  </si>
+  <si>
+    <t>Y0 = CF' + A'B'C' + BCE + BCD + A'C'D'E'F</t>
+  </si>
+  <si>
+    <t>Y2 = Y2 Y1' + Y2' Y1 TIM + Y2' Y1 CHQ</t>
+  </si>
+  <si>
+    <t>Y1 = Y1' Y0 BUT + Y2 Y1' BUT + Y2' Y1 CHQ' TIM'</t>
+  </si>
+  <si>
+    <t>Y0 = Y0 BUT' + Y2' Y1' Y0' + Y1 Y0 TIM + Y1 Y0 CHQ + Y2' Y0' CHQ' TIM' BUT</t>
+  </si>
+  <si>
+    <t>K = BC + A'B'C'</t>
+  </si>
+  <si>
+    <t>Z = AB'C'</t>
+  </si>
+  <si>
+    <t>W = AC</t>
+  </si>
+  <si>
+    <t>CLEAR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -242,8 +301,22 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -310,8 +383,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="22">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -606,12 +691,176 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -722,6 +971,99 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -1039,8 +1381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A4C429B-746C-4748-8FEA-F2B51B7B4385}">
   <dimension ref="A1:S64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3171,7 +3513,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M3" r:id="rId1" display="http://www.32x8.com/" xr:uid="{46987D7C-9D83-4F55-A4FB-FD555767C20F}"/>
+    <hyperlink ref="M3" r:id="rId1" xr:uid="{46987D7C-9D83-4F55-A4FB-FD555767C20F}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId2"/>
@@ -3183,7 +3525,7 @@
   <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="A10" sqref="A2:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3632,4 +3974,2641 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17577ADB-AED2-4E24-BA87-391E57BB5522}">
+  <dimension ref="A1:R66"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="8.21875" customWidth="1"/>
+    <col min="6" max="7" width="8.88671875" customWidth="1"/>
+    <col min="8" max="8" width="8" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5546875" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="0.33203125" customWidth="1"/>
+    <col min="13" max="13" width="38" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="63.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="77">
+        <v>0</v>
+      </c>
+      <c r="B3" s="69">
+        <v>0</v>
+      </c>
+      <c r="C3" s="22">
+        <v>0</v>
+      </c>
+      <c r="D3" s="62">
+        <v>0</v>
+      </c>
+      <c r="E3" s="85">
+        <v>0</v>
+      </c>
+      <c r="F3" s="86">
+        <v>0</v>
+      </c>
+      <c r="G3" s="87">
+        <v>0</v>
+      </c>
+      <c r="H3" s="67">
+        <v>0</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0</v>
+      </c>
+      <c r="J3" s="10">
+        <v>1</v>
+      </c>
+      <c r="K3" s="82" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="77">
+        <v>1</v>
+      </c>
+      <c r="B4" s="70">
+        <v>0</v>
+      </c>
+      <c r="C4" s="19">
+        <v>0</v>
+      </c>
+      <c r="D4" s="63">
+        <v>0</v>
+      </c>
+      <c r="E4" s="96">
+        <v>0</v>
+      </c>
+      <c r="F4" s="97">
+        <v>0</v>
+      </c>
+      <c r="G4" s="98">
+        <v>1</v>
+      </c>
+      <c r="H4" s="107">
+        <v>0</v>
+      </c>
+      <c r="I4" s="108">
+        <v>0</v>
+      </c>
+      <c r="J4" s="109">
+        <v>1</v>
+      </c>
+      <c r="K4" s="83"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="77">
+        <v>2</v>
+      </c>
+      <c r="B5" s="71">
+        <v>0</v>
+      </c>
+      <c r="C5" s="23">
+        <v>0</v>
+      </c>
+      <c r="D5" s="64">
+        <v>0</v>
+      </c>
+      <c r="E5" s="88">
+        <v>0</v>
+      </c>
+      <c r="F5" s="89">
+        <v>1</v>
+      </c>
+      <c r="G5" s="90">
+        <v>0</v>
+      </c>
+      <c r="H5" s="68">
+        <v>0</v>
+      </c>
+      <c r="I5" s="7">
+        <v>0</v>
+      </c>
+      <c r="J5" s="11">
+        <v>1</v>
+      </c>
+      <c r="K5" s="83"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="77">
+        <v>3</v>
+      </c>
+      <c r="B6" s="70">
+        <v>0</v>
+      </c>
+      <c r="C6" s="19">
+        <v>0</v>
+      </c>
+      <c r="D6" s="63">
+        <v>0</v>
+      </c>
+      <c r="E6" s="96">
+        <v>0</v>
+      </c>
+      <c r="F6" s="97">
+        <v>1</v>
+      </c>
+      <c r="G6" s="98">
+        <v>1</v>
+      </c>
+      <c r="H6" s="107">
+        <v>0</v>
+      </c>
+      <c r="I6" s="108">
+        <v>0</v>
+      </c>
+      <c r="J6" s="109">
+        <v>1</v>
+      </c>
+      <c r="K6" s="83"/>
+    </row>
+    <row r="7" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="77">
+        <v>4</v>
+      </c>
+      <c r="B7" s="71">
+        <v>0</v>
+      </c>
+      <c r="C7" s="23">
+        <v>0</v>
+      </c>
+      <c r="D7" s="64">
+        <v>0</v>
+      </c>
+      <c r="E7" s="88">
+        <v>1</v>
+      </c>
+      <c r="F7" s="89">
+        <v>0</v>
+      </c>
+      <c r="G7" s="90">
+        <v>0</v>
+      </c>
+      <c r="H7" s="68">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7">
+        <v>0</v>
+      </c>
+      <c r="J7" s="11">
+        <v>1</v>
+      </c>
+      <c r="K7" s="83"/>
+      <c r="M7" s="117" t="s">
+        <v>60</v>
+      </c>
+      <c r="N7" s="81" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="77">
+        <v>5</v>
+      </c>
+      <c r="B8" s="70">
+        <v>0</v>
+      </c>
+      <c r="C8" s="19">
+        <v>0</v>
+      </c>
+      <c r="D8" s="63">
+        <v>0</v>
+      </c>
+      <c r="E8" s="96">
+        <v>1</v>
+      </c>
+      <c r="F8" s="97">
+        <v>0</v>
+      </c>
+      <c r="G8" s="98">
+        <v>1</v>
+      </c>
+      <c r="H8" s="107">
+        <v>0</v>
+      </c>
+      <c r="I8" s="108">
+        <v>0</v>
+      </c>
+      <c r="J8" s="109">
+        <v>1</v>
+      </c>
+      <c r="K8" s="83"/>
+      <c r="M8" s="116" t="s">
+        <v>59</v>
+      </c>
+      <c r="N8" s="81" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="77">
+        <v>6</v>
+      </c>
+      <c r="B9" s="71">
+        <v>0</v>
+      </c>
+      <c r="C9" s="23">
+        <v>0</v>
+      </c>
+      <c r="D9" s="64">
+        <v>0</v>
+      </c>
+      <c r="E9" s="88">
+        <v>1</v>
+      </c>
+      <c r="F9" s="89">
+        <v>1</v>
+      </c>
+      <c r="G9" s="90">
+        <v>0</v>
+      </c>
+      <c r="H9" s="68">
+        <v>0</v>
+      </c>
+      <c r="I9" s="7">
+        <v>0</v>
+      </c>
+      <c r="J9" s="11">
+        <v>1</v>
+      </c>
+      <c r="K9" s="83"/>
+      <c r="M9" s="116" t="s">
+        <v>62</v>
+      </c>
+      <c r="N9" s="81" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="77">
+        <v>7</v>
+      </c>
+      <c r="B10" s="72">
+        <v>0</v>
+      </c>
+      <c r="C10" s="20">
+        <v>0</v>
+      </c>
+      <c r="D10" s="65">
+        <v>0</v>
+      </c>
+      <c r="E10" s="99">
+        <v>1</v>
+      </c>
+      <c r="F10" s="100">
+        <v>1</v>
+      </c>
+      <c r="G10" s="101">
+        <v>1</v>
+      </c>
+      <c r="H10" s="110">
+        <v>0</v>
+      </c>
+      <c r="I10" s="111">
+        <v>0</v>
+      </c>
+      <c r="J10" s="112">
+        <v>1</v>
+      </c>
+      <c r="K10" s="84"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="77">
+        <v>8</v>
+      </c>
+      <c r="B11" s="69">
+        <v>0</v>
+      </c>
+      <c r="C11" s="22">
+        <v>0</v>
+      </c>
+      <c r="D11" s="62">
+        <v>1</v>
+      </c>
+      <c r="E11" s="85">
+        <v>0</v>
+      </c>
+      <c r="F11" s="86">
+        <v>0</v>
+      </c>
+      <c r="G11" s="87">
+        <v>0</v>
+      </c>
+      <c r="H11" s="67">
+        <v>0</v>
+      </c>
+      <c r="I11" s="6">
+        <v>0</v>
+      </c>
+      <c r="J11" s="10">
+        <v>1</v>
+      </c>
+      <c r="K11" s="82" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="77">
+        <v>9</v>
+      </c>
+      <c r="B12" s="70">
+        <v>0</v>
+      </c>
+      <c r="C12" s="19">
+        <v>0</v>
+      </c>
+      <c r="D12" s="63">
+        <v>1</v>
+      </c>
+      <c r="E12" s="96">
+        <v>0</v>
+      </c>
+      <c r="F12" s="97">
+        <v>0</v>
+      </c>
+      <c r="G12" s="98">
+        <v>1</v>
+      </c>
+      <c r="H12" s="107">
+        <v>0</v>
+      </c>
+      <c r="I12" s="108">
+        <v>1</v>
+      </c>
+      <c r="J12" s="109">
+        <v>0</v>
+      </c>
+      <c r="K12" s="83"/>
+      <c r="N12" s="9"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="77">
+        <v>10</v>
+      </c>
+      <c r="B13" s="71">
+        <v>0</v>
+      </c>
+      <c r="C13" s="23">
+        <v>0</v>
+      </c>
+      <c r="D13" s="64">
+        <v>1</v>
+      </c>
+      <c r="E13" s="88">
+        <v>0</v>
+      </c>
+      <c r="F13" s="89">
+        <v>1</v>
+      </c>
+      <c r="G13" s="90">
+        <v>0</v>
+      </c>
+      <c r="H13" s="68">
+        <v>0</v>
+      </c>
+      <c r="I13" s="7">
+        <v>0</v>
+      </c>
+      <c r="J13" s="11">
+        <v>1</v>
+      </c>
+      <c r="K13" s="83"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="77">
+        <v>11</v>
+      </c>
+      <c r="B14" s="70">
+        <v>0</v>
+      </c>
+      <c r="C14" s="19">
+        <v>0</v>
+      </c>
+      <c r="D14" s="63">
+        <v>1</v>
+      </c>
+      <c r="E14" s="96">
+        <v>0</v>
+      </c>
+      <c r="F14" s="97">
+        <v>1</v>
+      </c>
+      <c r="G14" s="98">
+        <v>1</v>
+      </c>
+      <c r="H14" s="107">
+        <v>0</v>
+      </c>
+      <c r="I14" s="108">
+        <v>1</v>
+      </c>
+      <c r="J14" s="109">
+        <v>0</v>
+      </c>
+      <c r="K14" s="83"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="77">
+        <v>12</v>
+      </c>
+      <c r="B15" s="71">
+        <v>0</v>
+      </c>
+      <c r="C15" s="23">
+        <v>0</v>
+      </c>
+      <c r="D15" s="64">
+        <v>1</v>
+      </c>
+      <c r="E15" s="88">
+        <v>1</v>
+      </c>
+      <c r="F15" s="89">
+        <v>0</v>
+      </c>
+      <c r="G15" s="90">
+        <v>0</v>
+      </c>
+      <c r="H15" s="68">
+        <v>0</v>
+      </c>
+      <c r="I15" s="7">
+        <v>0</v>
+      </c>
+      <c r="J15" s="11">
+        <v>1</v>
+      </c>
+      <c r="K15" s="83"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="77">
+        <v>13</v>
+      </c>
+      <c r="B16" s="70">
+        <v>0</v>
+      </c>
+      <c r="C16" s="19">
+        <v>0</v>
+      </c>
+      <c r="D16" s="63">
+        <v>1</v>
+      </c>
+      <c r="E16" s="96">
+        <v>1</v>
+      </c>
+      <c r="F16" s="97">
+        <v>0</v>
+      </c>
+      <c r="G16" s="98">
+        <v>1</v>
+      </c>
+      <c r="H16" s="107">
+        <v>0</v>
+      </c>
+      <c r="I16" s="108">
+        <v>1</v>
+      </c>
+      <c r="J16" s="109">
+        <v>0</v>
+      </c>
+      <c r="K16" s="83"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A17" s="77">
+        <v>14</v>
+      </c>
+      <c r="B17" s="71">
+        <v>0</v>
+      </c>
+      <c r="C17" s="23">
+        <v>0</v>
+      </c>
+      <c r="D17" s="64">
+        <v>1</v>
+      </c>
+      <c r="E17" s="88">
+        <v>1</v>
+      </c>
+      <c r="F17" s="89">
+        <v>1</v>
+      </c>
+      <c r="G17" s="90">
+        <v>0</v>
+      </c>
+      <c r="H17" s="68">
+        <v>0</v>
+      </c>
+      <c r="I17" s="7">
+        <v>0</v>
+      </c>
+      <c r="J17" s="11">
+        <v>1</v>
+      </c>
+      <c r="K17" s="83"/>
+    </row>
+    <row r="18" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="77">
+        <v>15</v>
+      </c>
+      <c r="B18" s="72">
+        <v>0</v>
+      </c>
+      <c r="C18" s="20">
+        <v>0</v>
+      </c>
+      <c r="D18" s="65">
+        <v>1</v>
+      </c>
+      <c r="E18" s="99">
+        <v>1</v>
+      </c>
+      <c r="F18" s="100">
+        <v>1</v>
+      </c>
+      <c r="G18" s="101">
+        <v>1</v>
+      </c>
+      <c r="H18" s="110">
+        <v>0</v>
+      </c>
+      <c r="I18" s="111">
+        <v>1</v>
+      </c>
+      <c r="J18" s="112">
+        <v>0</v>
+      </c>
+      <c r="K18" s="84"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19" s="77">
+        <v>16</v>
+      </c>
+      <c r="B19" s="69">
+        <v>0</v>
+      </c>
+      <c r="C19" s="22">
+        <v>1</v>
+      </c>
+      <c r="D19" s="62">
+        <v>0</v>
+      </c>
+      <c r="E19" s="85">
+        <v>0</v>
+      </c>
+      <c r="F19" s="86">
+        <v>0</v>
+      </c>
+      <c r="G19" s="87">
+        <v>0</v>
+      </c>
+      <c r="H19" s="67">
+        <v>0</v>
+      </c>
+      <c r="I19" s="6">
+        <v>1</v>
+      </c>
+      <c r="J19" s="10">
+        <v>0</v>
+      </c>
+      <c r="K19" s="82" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A20" s="77">
+        <v>17</v>
+      </c>
+      <c r="B20" s="70">
+        <v>0</v>
+      </c>
+      <c r="C20" s="19">
+        <v>1</v>
+      </c>
+      <c r="D20" s="63">
+        <v>0</v>
+      </c>
+      <c r="E20" s="96">
+        <v>0</v>
+      </c>
+      <c r="F20" s="97">
+        <v>0</v>
+      </c>
+      <c r="G20" s="98">
+        <v>1</v>
+      </c>
+      <c r="H20" s="107">
+        <v>0</v>
+      </c>
+      <c r="I20" s="108">
+        <v>1</v>
+      </c>
+      <c r="J20" s="109">
+        <v>1</v>
+      </c>
+      <c r="K20" s="83"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A21" s="77">
+        <v>18</v>
+      </c>
+      <c r="B21" s="71">
+        <v>0</v>
+      </c>
+      <c r="C21" s="23">
+        <v>1</v>
+      </c>
+      <c r="D21" s="64">
+        <v>0</v>
+      </c>
+      <c r="E21" s="88">
+        <v>0</v>
+      </c>
+      <c r="F21" s="89">
+        <v>1</v>
+      </c>
+      <c r="G21" s="90">
+        <v>0</v>
+      </c>
+      <c r="H21" s="68">
+        <v>1</v>
+      </c>
+      <c r="I21" s="7">
+        <v>0</v>
+      </c>
+      <c r="J21" s="11">
+        <v>0</v>
+      </c>
+      <c r="K21" s="83"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A22" s="77">
+        <v>19</v>
+      </c>
+      <c r="B22" s="70">
+        <v>0</v>
+      </c>
+      <c r="C22" s="19">
+        <v>1</v>
+      </c>
+      <c r="D22" s="63">
+        <v>0</v>
+      </c>
+      <c r="E22" s="96">
+        <v>0</v>
+      </c>
+      <c r="F22" s="97">
+        <v>1</v>
+      </c>
+      <c r="G22" s="98">
+        <v>1</v>
+      </c>
+      <c r="H22" s="107">
+        <v>1</v>
+      </c>
+      <c r="I22" s="108">
+        <v>0</v>
+      </c>
+      <c r="J22" s="109">
+        <v>0</v>
+      </c>
+      <c r="K22" s="83"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A23" s="77">
+        <v>20</v>
+      </c>
+      <c r="B23" s="71">
+        <v>0</v>
+      </c>
+      <c r="C23" s="23">
+        <v>1</v>
+      </c>
+      <c r="D23" s="64">
+        <v>0</v>
+      </c>
+      <c r="E23" s="88">
+        <v>1</v>
+      </c>
+      <c r="F23" s="89">
+        <v>0</v>
+      </c>
+      <c r="G23" s="90">
+        <v>0</v>
+      </c>
+      <c r="H23" s="68">
+        <v>1</v>
+      </c>
+      <c r="I23" s="7">
+        <v>0</v>
+      </c>
+      <c r="J23" s="11">
+        <v>0</v>
+      </c>
+      <c r="K23" s="83"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A24" s="77">
+        <v>21</v>
+      </c>
+      <c r="B24" s="70">
+        <v>0</v>
+      </c>
+      <c r="C24" s="19">
+        <v>1</v>
+      </c>
+      <c r="D24" s="63">
+        <v>0</v>
+      </c>
+      <c r="E24" s="96">
+        <v>1</v>
+      </c>
+      <c r="F24" s="97">
+        <v>0</v>
+      </c>
+      <c r="G24" s="98">
+        <v>1</v>
+      </c>
+      <c r="H24" s="107">
+        <v>1</v>
+      </c>
+      <c r="I24" s="108">
+        <v>0</v>
+      </c>
+      <c r="J24" s="109">
+        <v>0</v>
+      </c>
+      <c r="K24" s="83"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A25" s="77">
+        <v>22</v>
+      </c>
+      <c r="B25" s="71">
+        <v>0</v>
+      </c>
+      <c r="C25" s="23">
+        <v>1</v>
+      </c>
+      <c r="D25" s="64">
+        <v>0</v>
+      </c>
+      <c r="E25" s="88">
+        <v>1</v>
+      </c>
+      <c r="F25" s="89">
+        <v>1</v>
+      </c>
+      <c r="G25" s="90">
+        <v>0</v>
+      </c>
+      <c r="H25" s="68">
+        <v>1</v>
+      </c>
+      <c r="I25" s="7">
+        <v>0</v>
+      </c>
+      <c r="J25" s="11">
+        <v>0</v>
+      </c>
+      <c r="K25" s="83"/>
+    </row>
+    <row r="26" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="77">
+        <v>23</v>
+      </c>
+      <c r="B26" s="72">
+        <v>0</v>
+      </c>
+      <c r="C26" s="20">
+        <v>1</v>
+      </c>
+      <c r="D26" s="65">
+        <v>0</v>
+      </c>
+      <c r="E26" s="99">
+        <v>1</v>
+      </c>
+      <c r="F26" s="100">
+        <v>1</v>
+      </c>
+      <c r="G26" s="101">
+        <v>1</v>
+      </c>
+      <c r="H26" s="110">
+        <v>1</v>
+      </c>
+      <c r="I26" s="111">
+        <v>0</v>
+      </c>
+      <c r="J26" s="112">
+        <v>0</v>
+      </c>
+      <c r="K26" s="84"/>
+      <c r="N26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O26" s="5">
+        <v>0</v>
+      </c>
+      <c r="P26" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="5">
+        <v>0</v>
+      </c>
+      <c r="R26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A27" s="77">
+        <v>24</v>
+      </c>
+      <c r="B27" s="69">
+        <v>0</v>
+      </c>
+      <c r="C27" s="22">
+        <v>1</v>
+      </c>
+      <c r="D27" s="62">
+        <v>1</v>
+      </c>
+      <c r="E27" s="85">
+        <v>0</v>
+      </c>
+      <c r="F27" s="86">
+        <v>0</v>
+      </c>
+      <c r="G27" s="87">
+        <v>0</v>
+      </c>
+      <c r="H27" s="67">
+        <v>0</v>
+      </c>
+      <c r="I27" s="6">
+        <v>1</v>
+      </c>
+      <c r="J27" s="10">
+        <v>1</v>
+      </c>
+      <c r="K27" s="82" t="s">
+        <v>54</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O27" s="5">
+        <v>0</v>
+      </c>
+      <c r="P27" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="5">
+        <v>1</v>
+      </c>
+      <c r="R27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A28" s="77">
+        <v>25</v>
+      </c>
+      <c r="B28" s="70">
+        <v>0</v>
+      </c>
+      <c r="C28" s="19">
+        <v>1</v>
+      </c>
+      <c r="D28" s="63">
+        <v>1</v>
+      </c>
+      <c r="E28" s="96">
+        <v>0</v>
+      </c>
+      <c r="F28" s="97">
+        <v>0</v>
+      </c>
+      <c r="G28" s="98">
+        <v>1</v>
+      </c>
+      <c r="H28" s="107">
+        <v>0</v>
+      </c>
+      <c r="I28" s="108">
+        <v>1</v>
+      </c>
+      <c r="J28" s="109">
+        <v>0</v>
+      </c>
+      <c r="K28" s="83"/>
+      <c r="N28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O28" s="5">
+        <v>0</v>
+      </c>
+      <c r="P28" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="5">
+        <v>0</v>
+      </c>
+      <c r="R28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A29" s="77">
+        <v>26</v>
+      </c>
+      <c r="B29" s="71">
+        <v>0</v>
+      </c>
+      <c r="C29" s="23">
+        <v>1</v>
+      </c>
+      <c r="D29" s="64">
+        <v>1</v>
+      </c>
+      <c r="E29" s="88">
+        <v>0</v>
+      </c>
+      <c r="F29" s="89">
+        <v>1</v>
+      </c>
+      <c r="G29" s="90">
+        <v>0</v>
+      </c>
+      <c r="H29" s="68">
+        <v>1</v>
+      </c>
+      <c r="I29" s="7">
+        <v>0</v>
+      </c>
+      <c r="J29" s="11">
+        <v>1</v>
+      </c>
+      <c r="K29" s="83"/>
+      <c r="N29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O29" s="5">
+        <v>0</v>
+      </c>
+      <c r="P29" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="5">
+        <v>1</v>
+      </c>
+      <c r="R29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A30" s="77">
+        <v>27</v>
+      </c>
+      <c r="B30" s="70">
+        <v>0</v>
+      </c>
+      <c r="C30" s="19">
+        <v>1</v>
+      </c>
+      <c r="D30" s="63">
+        <v>1</v>
+      </c>
+      <c r="E30" s="96">
+        <v>0</v>
+      </c>
+      <c r="F30" s="97">
+        <v>1</v>
+      </c>
+      <c r="G30" s="98">
+        <v>1</v>
+      </c>
+      <c r="H30" s="107">
+        <v>1</v>
+      </c>
+      <c r="I30" s="108">
+        <v>0</v>
+      </c>
+      <c r="J30" s="109">
+        <v>1</v>
+      </c>
+      <c r="K30" s="83"/>
+      <c r="N30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O30" s="5">
+        <v>1</v>
+      </c>
+      <c r="P30" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="5">
+        <v>0</v>
+      </c>
+      <c r="R30" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A31" s="77">
+        <v>28</v>
+      </c>
+      <c r="B31" s="71">
+        <v>0</v>
+      </c>
+      <c r="C31" s="23">
+        <v>1</v>
+      </c>
+      <c r="D31" s="64">
+        <v>1</v>
+      </c>
+      <c r="E31" s="88">
+        <v>1</v>
+      </c>
+      <c r="F31" s="89">
+        <v>0</v>
+      </c>
+      <c r="G31" s="90">
+        <v>0</v>
+      </c>
+      <c r="H31" s="68">
+        <v>1</v>
+      </c>
+      <c r="I31" s="7">
+        <v>0</v>
+      </c>
+      <c r="J31" s="11">
+        <v>1</v>
+      </c>
+      <c r="K31" s="83"/>
+      <c r="N31" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O31" s="5">
+        <v>1</v>
+      </c>
+      <c r="P31" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="5">
+        <v>1</v>
+      </c>
+      <c r="R31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A32" s="77">
+        <v>29</v>
+      </c>
+      <c r="B32" s="70">
+        <v>0</v>
+      </c>
+      <c r="C32" s="19">
+        <v>1</v>
+      </c>
+      <c r="D32" s="63">
+        <v>1</v>
+      </c>
+      <c r="E32" s="96">
+        <v>1</v>
+      </c>
+      <c r="F32" s="97">
+        <v>0</v>
+      </c>
+      <c r="G32" s="98">
+        <v>1</v>
+      </c>
+      <c r="H32" s="107">
+        <v>1</v>
+      </c>
+      <c r="I32" s="108">
+        <v>0</v>
+      </c>
+      <c r="J32" s="109">
+        <v>1</v>
+      </c>
+      <c r="K32" s="83"/>
+      <c r="N32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O32" s="5">
+        <v>1</v>
+      </c>
+      <c r="P32" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q32" s="5">
+        <v>0</v>
+      </c>
+      <c r="R32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A33" s="77">
+        <v>30</v>
+      </c>
+      <c r="B33" s="71">
+        <v>0</v>
+      </c>
+      <c r="C33" s="23">
+        <v>1</v>
+      </c>
+      <c r="D33" s="64">
+        <v>1</v>
+      </c>
+      <c r="E33" s="88">
+        <v>1</v>
+      </c>
+      <c r="F33" s="89">
+        <v>1</v>
+      </c>
+      <c r="G33" s="90">
+        <v>0</v>
+      </c>
+      <c r="H33" s="68">
+        <v>1</v>
+      </c>
+      <c r="I33" s="7">
+        <v>0</v>
+      </c>
+      <c r="J33" s="11">
+        <v>1</v>
+      </c>
+      <c r="K33" s="83"/>
+      <c r="N33" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O33" s="5">
+        <v>1</v>
+      </c>
+      <c r="P33" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="77">
+        <v>31</v>
+      </c>
+      <c r="B34" s="72">
+        <v>0</v>
+      </c>
+      <c r="C34" s="20">
+        <v>1</v>
+      </c>
+      <c r="D34" s="65">
+        <v>1</v>
+      </c>
+      <c r="E34" s="99">
+        <v>1</v>
+      </c>
+      <c r="F34" s="100">
+        <v>1</v>
+      </c>
+      <c r="G34" s="101">
+        <v>1</v>
+      </c>
+      <c r="H34" s="110">
+        <v>1</v>
+      </c>
+      <c r="I34" s="111">
+        <v>0</v>
+      </c>
+      <c r="J34" s="112">
+        <v>1</v>
+      </c>
+      <c r="K34" s="84"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A35" s="77">
+        <v>32</v>
+      </c>
+      <c r="B35" s="69">
+        <v>1</v>
+      </c>
+      <c r="C35" s="22">
+        <v>0</v>
+      </c>
+      <c r="D35" s="62">
+        <v>0</v>
+      </c>
+      <c r="E35" s="85">
+        <v>0</v>
+      </c>
+      <c r="F35" s="86">
+        <v>0</v>
+      </c>
+      <c r="G35" s="91">
+        <v>0</v>
+      </c>
+      <c r="H35" s="6">
+        <v>1</v>
+      </c>
+      <c r="I35" s="6">
+        <v>0</v>
+      </c>
+      <c r="J35" s="6">
+        <v>0</v>
+      </c>
+      <c r="K35" s="82" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A36" s="77">
+        <v>33</v>
+      </c>
+      <c r="B36" s="70">
+        <v>1</v>
+      </c>
+      <c r="C36" s="19">
+        <v>0</v>
+      </c>
+      <c r="D36" s="63">
+        <v>0</v>
+      </c>
+      <c r="E36" s="96">
+        <v>0</v>
+      </c>
+      <c r="F36" s="97">
+        <v>0</v>
+      </c>
+      <c r="G36" s="102">
+        <v>1</v>
+      </c>
+      <c r="H36" s="108">
+        <v>1</v>
+      </c>
+      <c r="I36" s="108">
+        <v>1</v>
+      </c>
+      <c r="J36" s="108">
+        <v>0</v>
+      </c>
+      <c r="K36" s="83"/>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A37" s="77">
+        <v>34</v>
+      </c>
+      <c r="B37" s="71">
+        <v>1</v>
+      </c>
+      <c r="C37" s="23">
+        <v>0</v>
+      </c>
+      <c r="D37" s="64">
+        <v>0</v>
+      </c>
+      <c r="E37" s="88">
+        <v>0</v>
+      </c>
+      <c r="F37" s="89">
+        <v>1</v>
+      </c>
+      <c r="G37" s="92">
+        <v>0</v>
+      </c>
+      <c r="H37" s="7">
+        <v>1</v>
+      </c>
+      <c r="I37" s="7">
+        <v>0</v>
+      </c>
+      <c r="J37" s="7">
+        <v>0</v>
+      </c>
+      <c r="K37" s="83"/>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A38" s="77">
+        <v>35</v>
+      </c>
+      <c r="B38" s="70">
+        <v>1</v>
+      </c>
+      <c r="C38" s="19">
+        <v>0</v>
+      </c>
+      <c r="D38" s="63">
+        <v>0</v>
+      </c>
+      <c r="E38" s="96">
+        <v>0</v>
+      </c>
+      <c r="F38" s="97">
+        <v>1</v>
+      </c>
+      <c r="G38" s="102">
+        <v>1</v>
+      </c>
+      <c r="H38" s="108">
+        <v>1</v>
+      </c>
+      <c r="I38" s="108">
+        <v>1</v>
+      </c>
+      <c r="J38" s="108">
+        <v>0</v>
+      </c>
+      <c r="K38" s="83"/>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A39" s="77">
+        <v>36</v>
+      </c>
+      <c r="B39" s="71">
+        <v>1</v>
+      </c>
+      <c r="C39" s="23">
+        <v>0</v>
+      </c>
+      <c r="D39" s="64">
+        <v>0</v>
+      </c>
+      <c r="E39" s="88">
+        <v>1</v>
+      </c>
+      <c r="F39" s="89">
+        <v>0</v>
+      </c>
+      <c r="G39" s="92">
+        <v>0</v>
+      </c>
+      <c r="H39" s="7">
+        <v>1</v>
+      </c>
+      <c r="I39" s="7">
+        <v>0</v>
+      </c>
+      <c r="J39" s="7">
+        <v>0</v>
+      </c>
+      <c r="K39" s="83"/>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A40" s="77">
+        <v>37</v>
+      </c>
+      <c r="B40" s="70">
+        <v>1</v>
+      </c>
+      <c r="C40" s="19">
+        <v>0</v>
+      </c>
+      <c r="D40" s="63">
+        <v>0</v>
+      </c>
+      <c r="E40" s="96">
+        <v>1</v>
+      </c>
+      <c r="F40" s="97">
+        <v>0</v>
+      </c>
+      <c r="G40" s="102">
+        <v>1</v>
+      </c>
+      <c r="H40" s="108">
+        <v>1</v>
+      </c>
+      <c r="I40" s="108">
+        <v>1</v>
+      </c>
+      <c r="J40" s="108">
+        <v>0</v>
+      </c>
+      <c r="K40" s="83"/>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A41" s="77">
+        <v>38</v>
+      </c>
+      <c r="B41" s="71">
+        <v>1</v>
+      </c>
+      <c r="C41" s="23">
+        <v>0</v>
+      </c>
+      <c r="D41" s="64">
+        <v>0</v>
+      </c>
+      <c r="E41" s="88">
+        <v>1</v>
+      </c>
+      <c r="F41" s="89">
+        <v>1</v>
+      </c>
+      <c r="G41" s="92">
+        <v>0</v>
+      </c>
+      <c r="H41" s="7">
+        <v>1</v>
+      </c>
+      <c r="I41" s="7">
+        <v>0</v>
+      </c>
+      <c r="J41" s="7">
+        <v>0</v>
+      </c>
+      <c r="K41" s="83"/>
+    </row>
+    <row r="42" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="77">
+        <v>39</v>
+      </c>
+      <c r="B42" s="73">
+        <v>1</v>
+      </c>
+      <c r="C42" s="21">
+        <v>0</v>
+      </c>
+      <c r="D42" s="66">
+        <v>0</v>
+      </c>
+      <c r="E42" s="103">
+        <v>1</v>
+      </c>
+      <c r="F42" s="104">
+        <v>1</v>
+      </c>
+      <c r="G42" s="105">
+        <v>1</v>
+      </c>
+      <c r="H42" s="113">
+        <v>1</v>
+      </c>
+      <c r="I42" s="113">
+        <v>1</v>
+      </c>
+      <c r="J42" s="113">
+        <v>0</v>
+      </c>
+      <c r="K42" s="84"/>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A43" s="77">
+        <v>40</v>
+      </c>
+      <c r="B43" s="69">
+        <v>1</v>
+      </c>
+      <c r="C43" s="22">
+        <v>0</v>
+      </c>
+      <c r="D43" s="62">
+        <v>1</v>
+      </c>
+      <c r="E43" s="85">
+        <v>0</v>
+      </c>
+      <c r="F43" s="86">
+        <v>0</v>
+      </c>
+      <c r="G43" s="91">
+        <v>0</v>
+      </c>
+      <c r="H43" s="6">
+        <v>1</v>
+      </c>
+      <c r="I43" s="6">
+        <v>0</v>
+      </c>
+      <c r="J43" s="6">
+        <v>1</v>
+      </c>
+      <c r="K43" s="82" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A44" s="77">
+        <v>41</v>
+      </c>
+      <c r="B44" s="70">
+        <v>1</v>
+      </c>
+      <c r="C44" s="19">
+        <v>0</v>
+      </c>
+      <c r="D44" s="63">
+        <v>1</v>
+      </c>
+      <c r="E44" s="96">
+        <v>0</v>
+      </c>
+      <c r="F44" s="97">
+        <v>0</v>
+      </c>
+      <c r="G44" s="102">
+        <v>1</v>
+      </c>
+      <c r="H44" s="108">
+        <v>1</v>
+      </c>
+      <c r="I44" s="108">
+        <v>1</v>
+      </c>
+      <c r="J44" s="108">
+        <v>0</v>
+      </c>
+      <c r="K44" s="83"/>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A45" s="77">
+        <v>42</v>
+      </c>
+      <c r="B45" s="71">
+        <v>1</v>
+      </c>
+      <c r="C45" s="23">
+        <v>0</v>
+      </c>
+      <c r="D45" s="64">
+        <v>1</v>
+      </c>
+      <c r="E45" s="88">
+        <v>0</v>
+      </c>
+      <c r="F45" s="89">
+        <v>1</v>
+      </c>
+      <c r="G45" s="92">
+        <v>0</v>
+      </c>
+      <c r="H45" s="7">
+        <v>1</v>
+      </c>
+      <c r="I45" s="7">
+        <v>0</v>
+      </c>
+      <c r="J45" s="7">
+        <v>1</v>
+      </c>
+      <c r="K45" s="83"/>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A46" s="77">
+        <v>43</v>
+      </c>
+      <c r="B46" s="70">
+        <v>1</v>
+      </c>
+      <c r="C46" s="19">
+        <v>0</v>
+      </c>
+      <c r="D46" s="63">
+        <v>1</v>
+      </c>
+      <c r="E46" s="96">
+        <v>0</v>
+      </c>
+      <c r="F46" s="97">
+        <v>1</v>
+      </c>
+      <c r="G46" s="102">
+        <v>1</v>
+      </c>
+      <c r="H46" s="108">
+        <v>1</v>
+      </c>
+      <c r="I46" s="108">
+        <v>1</v>
+      </c>
+      <c r="J46" s="108">
+        <v>0</v>
+      </c>
+      <c r="K46" s="83"/>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A47" s="77">
+        <v>44</v>
+      </c>
+      <c r="B47" s="71">
+        <v>1</v>
+      </c>
+      <c r="C47" s="23">
+        <v>0</v>
+      </c>
+      <c r="D47" s="64">
+        <v>1</v>
+      </c>
+      <c r="E47" s="88">
+        <v>1</v>
+      </c>
+      <c r="F47" s="89">
+        <v>0</v>
+      </c>
+      <c r="G47" s="92">
+        <v>0</v>
+      </c>
+      <c r="H47" s="7">
+        <v>1</v>
+      </c>
+      <c r="I47" s="7">
+        <v>0</v>
+      </c>
+      <c r="J47" s="7">
+        <v>1</v>
+      </c>
+      <c r="K47" s="83"/>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A48" s="77">
+        <v>45</v>
+      </c>
+      <c r="B48" s="70">
+        <v>1</v>
+      </c>
+      <c r="C48" s="19">
+        <v>0</v>
+      </c>
+      <c r="D48" s="63">
+        <v>1</v>
+      </c>
+      <c r="E48" s="96">
+        <v>1</v>
+      </c>
+      <c r="F48" s="97">
+        <v>0</v>
+      </c>
+      <c r="G48" s="102">
+        <v>1</v>
+      </c>
+      <c r="H48" s="108">
+        <v>1</v>
+      </c>
+      <c r="I48" s="108">
+        <v>1</v>
+      </c>
+      <c r="J48" s="108">
+        <v>0</v>
+      </c>
+      <c r="K48" s="83"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A49" s="77">
+        <v>46</v>
+      </c>
+      <c r="B49" s="71">
+        <v>1</v>
+      </c>
+      <c r="C49" s="23">
+        <v>0</v>
+      </c>
+      <c r="D49" s="64">
+        <v>1</v>
+      </c>
+      <c r="E49" s="88">
+        <v>1</v>
+      </c>
+      <c r="F49" s="89">
+        <v>1</v>
+      </c>
+      <c r="G49" s="92">
+        <v>0</v>
+      </c>
+      <c r="H49" s="7">
+        <v>1</v>
+      </c>
+      <c r="I49" s="7">
+        <v>0</v>
+      </c>
+      <c r="J49" s="7">
+        <v>1</v>
+      </c>
+      <c r="K49" s="83"/>
+    </row>
+    <row r="50" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="77">
+        <v>47</v>
+      </c>
+      <c r="B50" s="72">
+        <v>1</v>
+      </c>
+      <c r="C50" s="20">
+        <v>0</v>
+      </c>
+      <c r="D50" s="65">
+        <v>1</v>
+      </c>
+      <c r="E50" s="99">
+        <v>1</v>
+      </c>
+      <c r="F50" s="100">
+        <v>1</v>
+      </c>
+      <c r="G50" s="106">
+        <v>1</v>
+      </c>
+      <c r="H50" s="111">
+        <v>1</v>
+      </c>
+      <c r="I50" s="111">
+        <v>1</v>
+      </c>
+      <c r="J50" s="111">
+        <v>0</v>
+      </c>
+      <c r="K50" s="84"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A51" s="77">
+        <v>48</v>
+      </c>
+      <c r="B51" s="80">
+        <v>1</v>
+      </c>
+      <c r="C51" s="78">
+        <v>1</v>
+      </c>
+      <c r="D51" s="79">
+        <v>0</v>
+      </c>
+      <c r="E51" s="93">
+        <v>0</v>
+      </c>
+      <c r="F51" s="94">
+        <v>0</v>
+      </c>
+      <c r="G51" s="95">
+        <v>0</v>
+      </c>
+      <c r="H51" s="74">
+        <v>0</v>
+      </c>
+      <c r="I51" s="75">
+        <v>0</v>
+      </c>
+      <c r="J51" s="76">
+        <v>0</v>
+      </c>
+      <c r="K51" s="82" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A52" s="77">
+        <v>49</v>
+      </c>
+      <c r="B52" s="70">
+        <v>1</v>
+      </c>
+      <c r="C52" s="19">
+        <v>1</v>
+      </c>
+      <c r="D52" s="63">
+        <v>0</v>
+      </c>
+      <c r="E52" s="96">
+        <v>0</v>
+      </c>
+      <c r="F52" s="97">
+        <v>0</v>
+      </c>
+      <c r="G52" s="98">
+        <v>1</v>
+      </c>
+      <c r="H52" s="107">
+        <v>0</v>
+      </c>
+      <c r="I52" s="108">
+        <v>0</v>
+      </c>
+      <c r="J52" s="109">
+        <v>0</v>
+      </c>
+      <c r="K52" s="83"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A53" s="77">
+        <v>50</v>
+      </c>
+      <c r="B53" s="71">
+        <v>1</v>
+      </c>
+      <c r="C53" s="23">
+        <v>1</v>
+      </c>
+      <c r="D53" s="64">
+        <v>0</v>
+      </c>
+      <c r="E53" s="88">
+        <v>0</v>
+      </c>
+      <c r="F53" s="89">
+        <v>1</v>
+      </c>
+      <c r="G53" s="90">
+        <v>0</v>
+      </c>
+      <c r="H53" s="68">
+        <v>0</v>
+      </c>
+      <c r="I53" s="7">
+        <v>0</v>
+      </c>
+      <c r="J53" s="11">
+        <v>0</v>
+      </c>
+      <c r="K53" s="83"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A54" s="77">
+        <v>51</v>
+      </c>
+      <c r="B54" s="70">
+        <v>1</v>
+      </c>
+      <c r="C54" s="19">
+        <v>1</v>
+      </c>
+      <c r="D54" s="63">
+        <v>0</v>
+      </c>
+      <c r="E54" s="96">
+        <v>0</v>
+      </c>
+      <c r="F54" s="97">
+        <v>1</v>
+      </c>
+      <c r="G54" s="98">
+        <v>1</v>
+      </c>
+      <c r="H54" s="107">
+        <v>0</v>
+      </c>
+      <c r="I54" s="108">
+        <v>0</v>
+      </c>
+      <c r="J54" s="109">
+        <v>0</v>
+      </c>
+      <c r="K54" s="83"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A55" s="77">
+        <v>52</v>
+      </c>
+      <c r="B55" s="71">
+        <v>1</v>
+      </c>
+      <c r="C55" s="23">
+        <v>1</v>
+      </c>
+      <c r="D55" s="64">
+        <v>0</v>
+      </c>
+      <c r="E55" s="88">
+        <v>1</v>
+      </c>
+      <c r="F55" s="89">
+        <v>0</v>
+      </c>
+      <c r="G55" s="90">
+        <v>0</v>
+      </c>
+      <c r="H55" s="68">
+        <v>0</v>
+      </c>
+      <c r="I55" s="7">
+        <v>0</v>
+      </c>
+      <c r="J55" s="11">
+        <v>0</v>
+      </c>
+      <c r="K55" s="83"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A56" s="77">
+        <v>53</v>
+      </c>
+      <c r="B56" s="70">
+        <v>1</v>
+      </c>
+      <c r="C56" s="19">
+        <v>1</v>
+      </c>
+      <c r="D56" s="63">
+        <v>0</v>
+      </c>
+      <c r="E56" s="96">
+        <v>1</v>
+      </c>
+      <c r="F56" s="97">
+        <v>0</v>
+      </c>
+      <c r="G56" s="98">
+        <v>1</v>
+      </c>
+      <c r="H56" s="107">
+        <v>0</v>
+      </c>
+      <c r="I56" s="108">
+        <v>0</v>
+      </c>
+      <c r="J56" s="109">
+        <v>0</v>
+      </c>
+      <c r="K56" s="83"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A57" s="77">
+        <v>54</v>
+      </c>
+      <c r="B57" s="71">
+        <v>1</v>
+      </c>
+      <c r="C57" s="23">
+        <v>1</v>
+      </c>
+      <c r="D57" s="64">
+        <v>0</v>
+      </c>
+      <c r="E57" s="88">
+        <v>1</v>
+      </c>
+      <c r="F57" s="89">
+        <v>1</v>
+      </c>
+      <c r="G57" s="90">
+        <v>0</v>
+      </c>
+      <c r="H57" s="68">
+        <v>0</v>
+      </c>
+      <c r="I57" s="7">
+        <v>0</v>
+      </c>
+      <c r="J57" s="11">
+        <v>0</v>
+      </c>
+      <c r="K57" s="83"/>
+    </row>
+    <row r="58" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="77">
+        <v>55</v>
+      </c>
+      <c r="B58" s="72">
+        <v>1</v>
+      </c>
+      <c r="C58" s="20">
+        <v>1</v>
+      </c>
+      <c r="D58" s="65">
+        <v>0</v>
+      </c>
+      <c r="E58" s="99">
+        <v>1</v>
+      </c>
+      <c r="F58" s="100">
+        <v>1</v>
+      </c>
+      <c r="G58" s="101">
+        <v>1</v>
+      </c>
+      <c r="H58" s="110">
+        <v>0</v>
+      </c>
+      <c r="I58" s="111">
+        <v>0</v>
+      </c>
+      <c r="J58" s="112">
+        <v>0</v>
+      </c>
+      <c r="K58" s="84"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A59" s="77">
+        <v>56</v>
+      </c>
+      <c r="B59" s="80">
+        <v>1</v>
+      </c>
+      <c r="C59" s="78">
+        <v>1</v>
+      </c>
+      <c r="D59" s="79">
+        <v>1</v>
+      </c>
+      <c r="E59" s="93">
+        <v>0</v>
+      </c>
+      <c r="F59" s="94">
+        <v>0</v>
+      </c>
+      <c r="G59" s="95">
+        <v>0</v>
+      </c>
+      <c r="H59" s="74" t="s">
+        <v>14</v>
+      </c>
+      <c r="I59" s="75" t="s">
+        <v>14</v>
+      </c>
+      <c r="J59" s="76" t="s">
+        <v>14</v>
+      </c>
+      <c r="K59" s="82"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A60" s="77">
+        <v>57</v>
+      </c>
+      <c r="B60" s="70">
+        <v>1</v>
+      </c>
+      <c r="C60" s="19">
+        <v>1</v>
+      </c>
+      <c r="D60" s="63">
+        <v>1</v>
+      </c>
+      <c r="E60" s="96">
+        <v>0</v>
+      </c>
+      <c r="F60" s="97">
+        <v>0</v>
+      </c>
+      <c r="G60" s="98">
+        <v>1</v>
+      </c>
+      <c r="H60" s="107" t="s">
+        <v>14</v>
+      </c>
+      <c r="I60" s="108" t="s">
+        <v>14</v>
+      </c>
+      <c r="J60" s="109" t="s">
+        <v>14</v>
+      </c>
+      <c r="K60" s="83"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A61" s="77">
+        <v>58</v>
+      </c>
+      <c r="B61" s="71">
+        <v>1</v>
+      </c>
+      <c r="C61" s="23">
+        <v>1</v>
+      </c>
+      <c r="D61" s="64">
+        <v>1</v>
+      </c>
+      <c r="E61" s="88">
+        <v>0</v>
+      </c>
+      <c r="F61" s="89">
+        <v>1</v>
+      </c>
+      <c r="G61" s="90">
+        <v>0</v>
+      </c>
+      <c r="H61" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="I61" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J61" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="K61" s="83"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A62" s="77">
+        <v>59</v>
+      </c>
+      <c r="B62" s="70">
+        <v>1</v>
+      </c>
+      <c r="C62" s="19">
+        <v>1</v>
+      </c>
+      <c r="D62" s="63">
+        <v>1</v>
+      </c>
+      <c r="E62" s="96">
+        <v>0</v>
+      </c>
+      <c r="F62" s="97">
+        <v>1</v>
+      </c>
+      <c r="G62" s="98">
+        <v>1</v>
+      </c>
+      <c r="H62" s="107" t="s">
+        <v>14</v>
+      </c>
+      <c r="I62" s="108" t="s">
+        <v>14</v>
+      </c>
+      <c r="J62" s="109" t="s">
+        <v>14</v>
+      </c>
+      <c r="K62" s="83"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A63" s="77">
+        <v>60</v>
+      </c>
+      <c r="B63" s="71">
+        <v>1</v>
+      </c>
+      <c r="C63" s="23">
+        <v>1</v>
+      </c>
+      <c r="D63" s="64">
+        <v>1</v>
+      </c>
+      <c r="E63" s="88">
+        <v>1</v>
+      </c>
+      <c r="F63" s="89">
+        <v>0</v>
+      </c>
+      <c r="G63" s="90">
+        <v>0</v>
+      </c>
+      <c r="H63" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="I63" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J63" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="K63" s="83"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A64" s="77">
+        <v>61</v>
+      </c>
+      <c r="B64" s="70">
+        <v>1</v>
+      </c>
+      <c r="C64" s="19">
+        <v>1</v>
+      </c>
+      <c r="D64" s="63">
+        <v>1</v>
+      </c>
+      <c r="E64" s="96">
+        <v>1</v>
+      </c>
+      <c r="F64" s="97">
+        <v>0</v>
+      </c>
+      <c r="G64" s="98">
+        <v>1</v>
+      </c>
+      <c r="H64" s="107" t="s">
+        <v>14</v>
+      </c>
+      <c r="I64" s="108" t="s">
+        <v>14</v>
+      </c>
+      <c r="J64" s="109" t="s">
+        <v>14</v>
+      </c>
+      <c r="K64" s="83"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A65" s="77">
+        <v>62</v>
+      </c>
+      <c r="B65" s="71">
+        <v>1</v>
+      </c>
+      <c r="C65" s="23">
+        <v>1</v>
+      </c>
+      <c r="D65" s="64">
+        <v>1</v>
+      </c>
+      <c r="E65" s="88">
+        <v>1</v>
+      </c>
+      <c r="F65" s="89">
+        <v>1</v>
+      </c>
+      <c r="G65" s="90">
+        <v>0</v>
+      </c>
+      <c r="H65" s="107" t="s">
+        <v>14</v>
+      </c>
+      <c r="I65" s="108" t="s">
+        <v>14</v>
+      </c>
+      <c r="J65" s="109" t="s">
+        <v>14</v>
+      </c>
+      <c r="K65" s="83"/>
+    </row>
+    <row r="66" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="77">
+        <v>63</v>
+      </c>
+      <c r="B66" s="72">
+        <v>1</v>
+      </c>
+      <c r="C66" s="20">
+        <v>1</v>
+      </c>
+      <c r="D66" s="65">
+        <v>1</v>
+      </c>
+      <c r="E66" s="99">
+        <v>1</v>
+      </c>
+      <c r="F66" s="100">
+        <v>1</v>
+      </c>
+      <c r="G66" s="101">
+        <v>1</v>
+      </c>
+      <c r="H66" s="107" t="s">
+        <v>14</v>
+      </c>
+      <c r="I66" s="108" t="s">
+        <v>14</v>
+      </c>
+      <c r="J66" s="109" t="s">
+        <v>14</v>
+      </c>
+      <c r="K66" s="84"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="K43:K50"/>
+    <mergeCell ref="K51:K58"/>
+    <mergeCell ref="K59:K66"/>
+    <mergeCell ref="K3:K10"/>
+    <mergeCell ref="K11:K18"/>
+    <mergeCell ref="K19:K26"/>
+    <mergeCell ref="K27:K34"/>
+    <mergeCell ref="K35:K42"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A8F6C9E-3D6D-47E4-BADF-F5D3C04823CB}">
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="119" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="J2" s="114" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="43">
+        <v>0</v>
+      </c>
+      <c r="C3" s="34">
+        <v>0</v>
+      </c>
+      <c r="D3" s="34">
+        <v>0</v>
+      </c>
+      <c r="E3" s="38">
+        <v>1</v>
+      </c>
+      <c r="F3" s="39">
+        <v>1</v>
+      </c>
+      <c r="G3" s="39">
+        <v>0</v>
+      </c>
+      <c r="H3" s="39">
+        <v>0</v>
+      </c>
+      <c r="I3" s="120">
+        <v>0</v>
+      </c>
+      <c r="J3" s="115" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="44">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1</v>
+      </c>
+      <c r="E4" s="32">
+        <v>0</v>
+      </c>
+      <c r="F4" s="33">
+        <v>0</v>
+      </c>
+      <c r="G4" s="33">
+        <v>0</v>
+      </c>
+      <c r="H4" s="33">
+        <v>0</v>
+      </c>
+      <c r="I4" s="118">
+        <v>0</v>
+      </c>
+      <c r="J4" s="115" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="44">
+        <v>0</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="32">
+        <v>1</v>
+      </c>
+      <c r="F5" s="33">
+        <v>0</v>
+      </c>
+      <c r="G5" s="33">
+        <v>0</v>
+      </c>
+      <c r="H5" s="33">
+        <v>0</v>
+      </c>
+      <c r="I5" s="118">
+        <v>0</v>
+      </c>
+      <c r="J5" s="115" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="44">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5">
+        <v>1</v>
+      </c>
+      <c r="E6" s="32">
+        <v>0</v>
+      </c>
+      <c r="F6" s="33">
+        <v>1</v>
+      </c>
+      <c r="G6" s="33">
+        <v>0</v>
+      </c>
+      <c r="H6" s="33">
+        <v>0</v>
+      </c>
+      <c r="I6" s="118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="44">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0</v>
+      </c>
+      <c r="E7" s="32">
+        <v>0</v>
+      </c>
+      <c r="F7" s="33">
+        <v>0</v>
+      </c>
+      <c r="G7" s="33">
+        <v>1</v>
+      </c>
+      <c r="H7" s="33">
+        <v>0</v>
+      </c>
+      <c r="I7" s="118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="44">
+        <v>1</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5">
+        <v>1</v>
+      </c>
+      <c r="E8" s="32">
+        <v>0</v>
+      </c>
+      <c r="F8" s="33">
+        <v>0</v>
+      </c>
+      <c r="G8" s="33">
+        <v>0</v>
+      </c>
+      <c r="H8" s="33">
+        <v>1</v>
+      </c>
+      <c r="I8" s="118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="44">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0</v>
+      </c>
+      <c r="E9" s="32">
+        <v>0</v>
+      </c>
+      <c r="F9" s="33">
+        <v>0</v>
+      </c>
+      <c r="G9" s="33">
+        <v>0</v>
+      </c>
+      <c r="H9" s="33">
+        <v>0</v>
+      </c>
+      <c r="I9" s="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="44">
+        <v>1</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5">
+        <v>1</v>
+      </c>
+      <c r="E10" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="118" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>